<commit_message>
Variable "TestResultExcelFilePath" is removed from all the methods to make Output file as dynamic
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite MonthlyCatA201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite MonthlyCatA201819.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="12_ncr:500000_{F8AC1A6D-64BD-4489-96E3-6BC5C1EED5BB}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="4455" windowWidth="14340" xWindow="390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="90"/>
+    <workbookView activeTab="3" windowHeight="4455" windowWidth="14340" xWindow="390" yWindow="90"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="56">
   <si>
     <t>TC</t>
   </si>
@@ -109,9 +108,6 @@
     <t>FirstReportNameInApplication</t>
   </si>
   <si>
-    <t>TestResultExcelFilePath</t>
-  </si>
-  <si>
     <t>worksheetNo</t>
   </si>
   <si>
@@ -194,15 +190,12 @@
   </si>
   <si>
     <t>66,000.00</t>
-  </si>
-  <si>
-    <t>F:\\Automation_TestResults\\Payroll_Tax_NI_Directors_TestReports 201819\\201819 Payroll National Insurance calculation Test result.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -289,7 +282,7 @@
   <cellStyles count="3">
     <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
@@ -624,7 +617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -716,10 +709,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -758,13 +751,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -775,13 +768,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>16</v>
@@ -792,13 +785,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>16</v>
@@ -810,13 +803,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>16</v>
@@ -828,13 +821,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>16</v>
@@ -846,13 +839,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>16</v>
@@ -864,13 +857,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>16</v>
@@ -882,13 +875,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>16</v>
@@ -900,13 +893,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>16</v>
@@ -926,11 +919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,13 +935,12 @@
     <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="31.28515625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="40.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="64.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -977,352 +969,322 @@
         <v>29</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="36.6" r="2" s="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="36.6" r="2" s="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row ht="30" r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row ht="30" r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H3" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row ht="30" r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-    </row>
-    <row ht="30" r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H4" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+    </row>
+    <row ht="30" r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row ht="30" r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H5" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row ht="30" r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row ht="30" r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H6" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+    </row>
+    <row ht="30" r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-    </row>
-    <row ht="30" r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row ht="30" r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-    </row>
-    <row ht="30" r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H8" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+    </row>
+    <row ht="30" r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-    </row>
-    <row ht="30" r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H9" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row ht="30" r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-    </row>
-    <row ht="30" r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="H10" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A3:A10" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A3:A10"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
@@ -1330,11 +1292,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,13 +1308,12 @@
     <col min="5" max="5" customWidth="true" width="12.0" collapsed="true"/>
     <col min="6" max="6" customWidth="true" width="26.28515625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="42.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="64.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="27.6" r="1" s="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
@@ -1381,63 +1342,57 @@
         <v>29</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="K1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="35.25" r="2" s="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="35.25" r="2" s="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink display="https://xcdpayrolldemo--pydemoprsb.cs83.my.salesforce.com/a0b4E000001RuhY" r:id="rId1" ref="E2"/>
+    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A2"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>